<commit_message>
[Modified]: ABC file 4]
</commit_message>
<xml_diff>
--- a/Báo Cáo/Activity_bar_chart và bảng phân hệ/Activity-bar-chart.xlsx
+++ b/Báo Cáo/Activity_bar_chart và bảng phân hệ/Activity-bar-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Software-Technology\Báo Cáo\Activity_bar_chart và bảng phân hệ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63685917-2FC4-42E0-9709-BC9C25EB7F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC277DD7-2C2E-42C0-8F8F-B369484EF19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="183">
   <si>
     <t>Trình lập kế hoạch Dự án</t>
   </si>
@@ -604,6 +604,12 @@
   </si>
   <si>
     <t>BE: C.R.D Account</t>
+  </si>
+  <si>
+    <t>FE: lockAccount</t>
+  </si>
+  <si>
+    <t>BE: lockAccount</t>
   </si>
 </sst>
 </file>
@@ -17571,13 +17577,13 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BT180"/>
+  <dimension ref="A1:BT182"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="8" ySplit="5" topLeftCell="I108" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="8" ySplit="5" topLeftCell="I105" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C110" sqref="C110"/>
+      <selection pane="bottomRight" activeCell="J114" sqref="J114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1"/>
@@ -26545,7 +26551,7 @@
     <row r="109" spans="2:71" ht="36" customHeight="1">
       <c r="B109" s="96"/>
       <c r="C109" s="65" t="s">
-        <v>113</v>
+        <v>181</v>
       </c>
       <c r="D109" s="40"/>
       <c r="E109" s="41"/>
@@ -26624,8 +26630,8 @@
     </row>
     <row r="110" spans="2:71" ht="36" customHeight="1">
       <c r="B110" s="96"/>
-      <c r="C110" s="60" t="s">
-        <v>180</v>
+      <c r="C110" s="65" t="s">
+        <v>113</v>
       </c>
       <c r="D110" s="40"/>
       <c r="E110" s="41"/>
@@ -26705,7 +26711,7 @@
     <row r="111" spans="2:71" ht="36" customHeight="1">
       <c r="B111" s="96"/>
       <c r="C111" s="60" t="s">
-        <v>61</v>
+        <v>180</v>
       </c>
       <c r="D111" s="40"/>
       <c r="E111" s="41"/>
@@ -26785,7 +26791,7 @@
     <row r="112" spans="2:71" ht="36" customHeight="1">
       <c r="B112" s="96"/>
       <c r="C112" s="60" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="D112" s="40"/>
       <c r="E112" s="41"/>
@@ -26865,7 +26871,7 @@
     <row r="113" spans="2:71" ht="36" customHeight="1">
       <c r="B113" s="96"/>
       <c r="C113" s="60" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D113" s="40"/>
       <c r="E113" s="41"/>
@@ -26942,20 +26948,20 @@
       <c r="BR113" s="4"/>
       <c r="BS113" s="4"/>
     </row>
-    <row r="114" spans="2:71" ht="36" customHeight="1" thickBot="1">
+    <row r="114" spans="2:71" ht="36" customHeight="1">
       <c r="B114" s="96"/>
-      <c r="C114" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D114" s="54"/>
-      <c r="E114" s="55"/>
-      <c r="F114" s="56">
+      <c r="C114" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="D114" s="40"/>
+      <c r="E114" s="41"/>
+      <c r="F114" s="42">
         <v>34</v>
       </c>
-      <c r="G114" s="56">
+      <c r="G114" s="42">
         <v>7</v>
       </c>
-      <c r="H114" s="57">
+      <c r="H114" s="45">
         <v>0</v>
       </c>
       <c r="I114" s="3"/>
@@ -27022,24 +27028,20 @@
       <c r="BR114" s="4"/>
       <c r="BS114" s="4"/>
     </row>
-    <row r="115" spans="2:71" ht="36" customHeight="1" thickTop="1">
-      <c r="B115" s="97"/>
-      <c r="C115" s="98" t="s">
-        <v>115</v>
-      </c>
-      <c r="D115" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="E115" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="F115" s="48">
+    <row r="115" spans="2:71" ht="36" customHeight="1">
+      <c r="B115" s="96"/>
+      <c r="C115" s="60" t="s">
+        <v>114</v>
+      </c>
+      <c r="D115" s="40"/>
+      <c r="E115" s="41"/>
+      <c r="F115" s="42">
         <v>34</v>
       </c>
-      <c r="G115" s="48">
+      <c r="G115" s="42">
         <v>7</v>
       </c>
-      <c r="H115" s="49">
+      <c r="H115" s="45">
         <v>0</v>
       </c>
       <c r="I115" s="3"/>
@@ -27106,20 +27108,20 @@
       <c r="BR115" s="4"/>
       <c r="BS115" s="4"/>
     </row>
-    <row r="116" spans="2:71" ht="36" customHeight="1">
-      <c r="B116" s="99"/>
-      <c r="C116" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="D116" s="40"/>
-      <c r="E116" s="41"/>
-      <c r="F116" s="42">
+    <row r="116" spans="2:71" ht="36" customHeight="1" thickBot="1">
+      <c r="B116" s="96"/>
+      <c r="C116" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D116" s="54"/>
+      <c r="E116" s="55"/>
+      <c r="F116" s="56">
         <v>34</v>
       </c>
-      <c r="G116" s="42">
+      <c r="G116" s="56">
         <v>7</v>
       </c>
-      <c r="H116" s="45">
+      <c r="H116" s="57">
         <v>0</v>
       </c>
       <c r="I116" s="3"/>
@@ -27186,20 +27188,24 @@
       <c r="BR116" s="4"/>
       <c r="BS116" s="4"/>
     </row>
-    <row r="117" spans="2:71" ht="36" customHeight="1">
-      <c r="B117" s="99"/>
-      <c r="C117" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="D117" s="40"/>
-      <c r="E117" s="41"/>
-      <c r="F117" s="42">
+    <row r="117" spans="2:71" ht="36" customHeight="1" thickTop="1">
+      <c r="B117" s="97"/>
+      <c r="C117" s="98" t="s">
+        <v>115</v>
+      </c>
+      <c r="D117" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="E117" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="F117" s="48">
         <v>34</v>
       </c>
-      <c r="G117" s="42">
+      <c r="G117" s="48">
         <v>7</v>
       </c>
-      <c r="H117" s="45">
+      <c r="H117" s="49">
         <v>0</v>
       </c>
       <c r="I117" s="3"/>
@@ -27269,7 +27275,7 @@
     <row r="118" spans="2:71" ht="36" customHeight="1">
       <c r="B118" s="99"/>
       <c r="C118" s="65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D118" s="40"/>
       <c r="E118" s="41"/>
@@ -27349,7 +27355,7 @@
     <row r="119" spans="2:71" ht="36" customHeight="1">
       <c r="B119" s="99"/>
       <c r="C119" s="65" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
       <c r="D119" s="40"/>
       <c r="E119" s="41"/>
@@ -27429,7 +27435,7 @@
     <row r="120" spans="2:71" ht="36" customHeight="1">
       <c r="B120" s="99"/>
       <c r="C120" s="65" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D120" s="40"/>
       <c r="E120" s="41"/>
@@ -27508,8 +27514,8 @@
     </row>
     <row r="121" spans="2:71" ht="36" customHeight="1">
       <c r="B121" s="99"/>
-      <c r="C121" s="60" t="s">
-        <v>119</v>
+      <c r="C121" s="65" t="s">
+        <v>118</v>
       </c>
       <c r="D121" s="40"/>
       <c r="E121" s="41"/>
@@ -27588,8 +27594,8 @@
     </row>
     <row r="122" spans="2:71" ht="36" customHeight="1">
       <c r="B122" s="99"/>
-      <c r="C122" s="60" t="s">
-        <v>61</v>
+      <c r="C122" s="65" t="s">
+        <v>122</v>
       </c>
       <c r="D122" s="40"/>
       <c r="E122" s="41"/>
@@ -27669,7 +27675,7 @@
     <row r="123" spans="2:71" ht="36" customHeight="1">
       <c r="B123" s="99"/>
       <c r="C123" s="60" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D123" s="40"/>
       <c r="E123" s="41"/>
@@ -27749,7 +27755,7 @@
     <row r="124" spans="2:71" ht="36" customHeight="1">
       <c r="B124" s="99"/>
       <c r="C124" s="60" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
       <c r="D124" s="40"/>
       <c r="E124" s="41"/>
@@ -27829,7 +27835,7 @@
     <row r="125" spans="2:71" ht="36" customHeight="1">
       <c r="B125" s="99"/>
       <c r="C125" s="60" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D125" s="40"/>
       <c r="E125" s="41"/>
@@ -27906,23 +27912,23 @@
       <c r="BR125" s="4"/>
       <c r="BS125" s="4"/>
     </row>
-    <row r="126" spans="2:71" ht="36" customHeight="1" thickBot="1">
-      <c r="B126" s="100"/>
-      <c r="C126" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D126" s="54"/>
-      <c r="E126" s="55"/>
-      <c r="F126" s="56">
+    <row r="126" spans="2:71" ht="36" customHeight="1">
+      <c r="B126" s="99"/>
+      <c r="C126" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="D126" s="40"/>
+      <c r="E126" s="41"/>
+      <c r="F126" s="42">
         <v>34</v>
       </c>
-      <c r="G126" s="56">
+      <c r="G126" s="42">
         <v>7</v>
       </c>
-      <c r="H126" s="57">
+      <c r="H126" s="45">
         <v>0</v>
       </c>
-      <c r="I126" s="67"/>
+      <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
@@ -27986,24 +27992,20 @@
       <c r="BR126" s="4"/>
       <c r="BS126" s="4"/>
     </row>
-    <row r="127" spans="2:71" ht="36" customHeight="1" thickTop="1">
-      <c r="B127" s="102"/>
-      <c r="C127" s="105" t="s">
-        <v>124</v>
-      </c>
-      <c r="D127" s="46" t="s">
+    <row r="127" spans="2:71" ht="36" customHeight="1">
+      <c r="B127" s="99"/>
+      <c r="C127" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="D127" s="40"/>
+      <c r="E127" s="41"/>
+      <c r="F127" s="42">
         <v>34</v>
       </c>
-      <c r="E127" s="47" t="s">
-        <v>165</v>
-      </c>
-      <c r="F127" s="48">
-        <v>34</v>
-      </c>
-      <c r="G127" s="48">
+      <c r="G127" s="42">
         <v>7</v>
       </c>
-      <c r="H127" s="49">
+      <c r="H127" s="45">
         <v>0</v>
       </c>
       <c r="I127" s="3"/>
@@ -28070,23 +28072,23 @@
       <c r="BR127" s="4"/>
       <c r="BS127" s="4"/>
     </row>
-    <row r="128" spans="2:71" ht="36" customHeight="1">
-      <c r="B128" s="103"/>
-      <c r="C128" s="65" t="s">
-        <v>125</v>
-      </c>
-      <c r="D128" s="40"/>
-      <c r="E128" s="41"/>
-      <c r="F128" s="42">
+    <row r="128" spans="2:71" ht="36" customHeight="1" thickBot="1">
+      <c r="B128" s="100"/>
+      <c r="C128" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D128" s="54"/>
+      <c r="E128" s="55"/>
+      <c r="F128" s="56">
         <v>34</v>
       </c>
-      <c r="G128" s="42">
+      <c r="G128" s="56">
         <v>7</v>
       </c>
-      <c r="H128" s="45">
+      <c r="H128" s="57">
         <v>0</v>
       </c>
-      <c r="I128" s="3"/>
+      <c r="I128" s="67"/>
       <c r="J128" s="3"/>
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
@@ -28150,20 +28152,24 @@
       <c r="BR128" s="4"/>
       <c r="BS128" s="4"/>
     </row>
-    <row r="129" spans="2:71" ht="36" customHeight="1">
-      <c r="B129" s="103"/>
-      <c r="C129" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="D129" s="40"/>
-      <c r="E129" s="41"/>
-      <c r="F129" s="42">
+    <row r="129" spans="2:71" ht="36" customHeight="1" thickTop="1">
+      <c r="B129" s="102"/>
+      <c r="C129" s="105" t="s">
+        <v>124</v>
+      </c>
+      <c r="D129" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="G129" s="42">
+      <c r="E129" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="F129" s="48">
+        <v>34</v>
+      </c>
+      <c r="G129" s="48">
         <v>7</v>
       </c>
-      <c r="H129" s="45">
+      <c r="H129" s="49">
         <v>0</v>
       </c>
       <c r="I129" s="3"/>
@@ -28233,7 +28239,7 @@
     <row r="130" spans="2:71" ht="36" customHeight="1">
       <c r="B130" s="103"/>
       <c r="C130" s="65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D130" s="40"/>
       <c r="E130" s="41"/>
@@ -28313,7 +28319,7 @@
     <row r="131" spans="2:71" ht="36" customHeight="1">
       <c r="B131" s="103"/>
       <c r="C131" s="65" t="s">
-        <v>127</v>
+        <v>53</v>
       </c>
       <c r="D131" s="40"/>
       <c r="E131" s="41"/>
@@ -28392,8 +28398,8 @@
     </row>
     <row r="132" spans="2:71" ht="36" customHeight="1">
       <c r="B132" s="103"/>
-      <c r="C132" s="60" t="s">
-        <v>128</v>
+      <c r="C132" s="65" t="s">
+        <v>126</v>
       </c>
       <c r="D132" s="40"/>
       <c r="E132" s="41"/>
@@ -28472,8 +28478,8 @@
     </row>
     <row r="133" spans="2:71" ht="36" customHeight="1">
       <c r="B133" s="103"/>
-      <c r="C133" s="60" t="s">
-        <v>61</v>
+      <c r="C133" s="65" t="s">
+        <v>127</v>
       </c>
       <c r="D133" s="40"/>
       <c r="E133" s="41"/>
@@ -28553,7 +28559,7 @@
     <row r="134" spans="2:71" ht="36" customHeight="1">
       <c r="B134" s="103"/>
       <c r="C134" s="60" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D134" s="40"/>
       <c r="E134" s="41"/>
@@ -28633,7 +28639,7 @@
     <row r="135" spans="2:71" ht="36" customHeight="1">
       <c r="B135" s="103"/>
       <c r="C135" s="60" t="s">
-        <v>146</v>
+        <v>61</v>
       </c>
       <c r="D135" s="40"/>
       <c r="E135" s="41"/>
@@ -28710,20 +28716,20 @@
       <c r="BR135" s="4"/>
       <c r="BS135" s="4"/>
     </row>
-    <row r="136" spans="2:71" ht="36" customHeight="1" thickBot="1">
-      <c r="B136" s="104"/>
-      <c r="C136" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D136" s="54"/>
-      <c r="E136" s="55"/>
-      <c r="F136" s="56">
+    <row r="136" spans="2:71" ht="36" customHeight="1">
+      <c r="B136" s="103"/>
+      <c r="C136" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="D136" s="40"/>
+      <c r="E136" s="41"/>
+      <c r="F136" s="42">
         <v>34</v>
       </c>
-      <c r="G136" s="56">
+      <c r="G136" s="42">
         <v>7</v>
       </c>
-      <c r="H136" s="57">
+      <c r="H136" s="45">
         <v>0</v>
       </c>
       <c r="I136" s="3"/>
@@ -28790,24 +28796,20 @@
       <c r="BR136" s="4"/>
       <c r="BS136" s="4"/>
     </row>
-    <row r="137" spans="2:71" ht="36" customHeight="1" thickTop="1">
-      <c r="B137" s="106"/>
-      <c r="C137" s="107" t="s">
-        <v>130</v>
-      </c>
-      <c r="D137" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="E137" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="F137" s="48">
-        <v>41</v>
-      </c>
-      <c r="G137" s="48">
-        <v>10</v>
-      </c>
-      <c r="H137" s="49">
+    <row r="137" spans="2:71" ht="36" customHeight="1">
+      <c r="B137" s="103"/>
+      <c r="C137" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="D137" s="40"/>
+      <c r="E137" s="41"/>
+      <c r="F137" s="42">
+        <v>34</v>
+      </c>
+      <c r="G137" s="42">
+        <v>7</v>
+      </c>
+      <c r="H137" s="45">
         <v>0</v>
       </c>
       <c r="I137" s="3"/>
@@ -28874,20 +28876,20 @@
       <c r="BR137" s="4"/>
       <c r="BS137" s="4"/>
     </row>
-    <row r="138" spans="2:71" ht="36" customHeight="1">
-      <c r="B138" s="108"/>
-      <c r="C138" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="D138" s="40"/>
-      <c r="E138" s="41"/>
-      <c r="F138" s="42">
-        <v>41</v>
-      </c>
-      <c r="G138" s="42">
-        <v>10</v>
-      </c>
-      <c r="H138" s="45">
+    <row r="138" spans="2:71" ht="36" customHeight="1" thickBot="1">
+      <c r="B138" s="104"/>
+      <c r="C138" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D138" s="54"/>
+      <c r="E138" s="55"/>
+      <c r="F138" s="56">
+        <v>34</v>
+      </c>
+      <c r="G138" s="56">
+        <v>7</v>
+      </c>
+      <c r="H138" s="57">
         <v>0</v>
       </c>
       <c r="I138" s="3"/>
@@ -28954,20 +28956,24 @@
       <c r="BR138" s="4"/>
       <c r="BS138" s="4"/>
     </row>
-    <row r="139" spans="2:71" ht="36" customHeight="1">
-      <c r="B139" s="108"/>
-      <c r="C139" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="D139" s="40"/>
-      <c r="E139" s="41"/>
-      <c r="F139" s="42">
+    <row r="139" spans="2:71" ht="36" customHeight="1" thickTop="1">
+      <c r="B139" s="106"/>
+      <c r="C139" s="107" t="s">
+        <v>130</v>
+      </c>
+      <c r="D139" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E139" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="F139" s="48">
         <v>41</v>
       </c>
-      <c r="G139" s="42">
+      <c r="G139" s="48">
         <v>10</v>
       </c>
-      <c r="H139" s="45">
+      <c r="H139" s="49">
         <v>0</v>
       </c>
       <c r="I139" s="3"/>
@@ -29037,7 +29043,7 @@
     <row r="140" spans="2:71" ht="36" customHeight="1">
       <c r="B140" s="108"/>
       <c r="C140" s="65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D140" s="40"/>
       <c r="E140" s="41"/>
@@ -29117,7 +29123,7 @@
     <row r="141" spans="2:71" ht="36" customHeight="1">
       <c r="B141" s="108"/>
       <c r="C141" s="65" t="s">
-        <v>134</v>
+        <v>53</v>
       </c>
       <c r="D141" s="40"/>
       <c r="E141" s="41"/>
@@ -29197,7 +29203,7 @@
     <row r="142" spans="2:71" ht="36" customHeight="1">
       <c r="B142" s="108"/>
       <c r="C142" s="65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D142" s="40"/>
       <c r="E142" s="41"/>
@@ -29276,8 +29282,8 @@
     </row>
     <row r="143" spans="2:71" ht="36" customHeight="1">
       <c r="B143" s="108"/>
-      <c r="C143" s="60" t="s">
-        <v>136</v>
+      <c r="C143" s="65" t="s">
+        <v>134</v>
       </c>
       <c r="D143" s="40"/>
       <c r="E143" s="41"/>
@@ -29356,8 +29362,8 @@
     </row>
     <row r="144" spans="2:71" ht="36" customHeight="1">
       <c r="B144" s="108"/>
-      <c r="C144" s="60" t="s">
-        <v>61</v>
+      <c r="C144" s="65" t="s">
+        <v>135</v>
       </c>
       <c r="D144" s="40"/>
       <c r="E144" s="41"/>
@@ -29434,10 +29440,10 @@
       <c r="BR144" s="4"/>
       <c r="BS144" s="4"/>
     </row>
-    <row r="145" spans="1:71" ht="36" customHeight="1">
+    <row r="145" spans="2:71" ht="36" customHeight="1">
       <c r="B145" s="108"/>
       <c r="C145" s="60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D145" s="40"/>
       <c r="E145" s="41"/>
@@ -29514,10 +29520,10 @@
       <c r="BR145" s="4"/>
       <c r="BS145" s="4"/>
     </row>
-    <row r="146" spans="1:71" ht="36" customHeight="1">
+    <row r="146" spans="2:71" ht="36" customHeight="1">
       <c r="B146" s="108"/>
       <c r="C146" s="60" t="s">
-        <v>138</v>
+        <v>61</v>
       </c>
       <c r="D146" s="40"/>
       <c r="E146" s="41"/>
@@ -29594,10 +29600,10 @@
       <c r="BR146" s="4"/>
       <c r="BS146" s="4"/>
     </row>
-    <row r="147" spans="1:71" ht="36" customHeight="1">
+    <row r="147" spans="2:71" ht="36" customHeight="1">
       <c r="B147" s="108"/>
       <c r="C147" s="60" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D147" s="40"/>
       <c r="E147" s="41"/>
@@ -29674,23 +29680,23 @@
       <c r="BR147" s="4"/>
       <c r="BS147" s="4"/>
     </row>
-    <row r="148" spans="1:71" ht="36" customHeight="1" thickBot="1">
-      <c r="B148" s="109"/>
-      <c r="C148" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D148" s="54"/>
-      <c r="E148" s="55"/>
-      <c r="F148" s="56">
+    <row r="148" spans="2:71" ht="36" customHeight="1">
+      <c r="B148" s="108"/>
+      <c r="C148" s="60" t="s">
+        <v>138</v>
+      </c>
+      <c r="D148" s="40"/>
+      <c r="E148" s="41"/>
+      <c r="F148" s="42">
         <v>41</v>
       </c>
-      <c r="G148" s="56">
+      <c r="G148" s="42">
         <v>10</v>
       </c>
-      <c r="H148" s="57">
+      <c r="H148" s="45">
         <v>0</v>
       </c>
-      <c r="I148" s="67"/>
+      <c r="I148" s="3"/>
       <c r="J148" s="3"/>
       <c r="K148" s="3"/>
       <c r="L148" s="3"/>
@@ -29754,24 +29760,20 @@
       <c r="BR148" s="4"/>
       <c r="BS148" s="4"/>
     </row>
-    <row r="149" spans="1:71" ht="36" customHeight="1" thickTop="1">
-      <c r="B149" s="110"/>
-      <c r="C149" s="111" t="s">
-        <v>131</v>
-      </c>
-      <c r="D149" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="E149" s="47" t="s">
-        <v>165</v>
-      </c>
-      <c r="F149" s="48">
+    <row r="149" spans="2:71" ht="36" customHeight="1">
+      <c r="B149" s="108"/>
+      <c r="C149" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="D149" s="40"/>
+      <c r="E149" s="41"/>
+      <c r="F149" s="42">
         <v>41</v>
       </c>
-      <c r="G149" s="48">
+      <c r="G149" s="42">
         <v>10</v>
       </c>
-      <c r="H149" s="49">
+      <c r="H149" s="45">
         <v>0</v>
       </c>
       <c r="I149" s="3"/>
@@ -29838,23 +29840,23 @@
       <c r="BR149" s="4"/>
       <c r="BS149" s="4"/>
     </row>
-    <row r="150" spans="1:71" ht="36" customHeight="1">
-      <c r="B150" s="112"/>
-      <c r="C150" s="65" t="s">
-        <v>140</v>
-      </c>
-      <c r="D150" s="40"/>
-      <c r="E150" s="41"/>
-      <c r="F150" s="42">
+    <row r="150" spans="2:71" ht="36" customHeight="1" thickBot="1">
+      <c r="B150" s="109"/>
+      <c r="C150" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D150" s="54"/>
+      <c r="E150" s="55"/>
+      <c r="F150" s="56">
         <v>41</v>
       </c>
-      <c r="G150" s="42">
+      <c r="G150" s="56">
         <v>10</v>
       </c>
-      <c r="H150" s="45">
+      <c r="H150" s="57">
         <v>0</v>
       </c>
-      <c r="I150" s="3"/>
+      <c r="I150" s="67"/>
       <c r="J150" s="3"/>
       <c r="K150" s="3"/>
       <c r="L150" s="3"/>
@@ -29918,20 +29920,24 @@
       <c r="BR150" s="4"/>
       <c r="BS150" s="4"/>
     </row>
-    <row r="151" spans="1:71" ht="36" customHeight="1">
-      <c r="B151" s="112"/>
-      <c r="C151" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="D151" s="40"/>
-      <c r="E151" s="41"/>
-      <c r="F151" s="42">
+    <row r="151" spans="2:71" ht="36" customHeight="1" thickTop="1">
+      <c r="B151" s="110"/>
+      <c r="C151" s="111" t="s">
+        <v>131</v>
+      </c>
+      <c r="D151" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="E151" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="F151" s="48">
         <v>41</v>
       </c>
-      <c r="G151" s="42">
+      <c r="G151" s="48">
         <v>10</v>
       </c>
-      <c r="H151" s="45">
+      <c r="H151" s="49">
         <v>0</v>
       </c>
       <c r="I151" s="3"/>
@@ -29998,10 +30004,10 @@
       <c r="BR151" s="4"/>
       <c r="BS151" s="4"/>
     </row>
-    <row r="152" spans="1:71" ht="36" customHeight="1">
+    <row r="152" spans="2:71" ht="36" customHeight="1">
       <c r="B152" s="112"/>
       <c r="C152" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D152" s="40"/>
       <c r="E152" s="41"/>
@@ -30078,10 +30084,10 @@
       <c r="BR152" s="4"/>
       <c r="BS152" s="4"/>
     </row>
-    <row r="153" spans="1:71" ht="36" customHeight="1">
+    <row r="153" spans="2:71" ht="36" customHeight="1">
       <c r="B153" s="112"/>
       <c r="C153" s="65" t="s">
-        <v>142</v>
+        <v>53</v>
       </c>
       <c r="D153" s="40"/>
       <c r="E153" s="41"/>
@@ -30158,10 +30164,10 @@
       <c r="BR153" s="4"/>
       <c r="BS153" s="4"/>
     </row>
-    <row r="154" spans="1:71" ht="36" customHeight="1">
+    <row r="154" spans="2:71" ht="36" customHeight="1">
       <c r="B154" s="112"/>
-      <c r="C154" s="60" t="s">
-        <v>143</v>
+      <c r="C154" s="65" t="s">
+        <v>141</v>
       </c>
       <c r="D154" s="40"/>
       <c r="E154" s="41"/>
@@ -30238,10 +30244,10 @@
       <c r="BR154" s="4"/>
       <c r="BS154" s="4"/>
     </row>
-    <row r="155" spans="1:71" ht="36" customHeight="1">
+    <row r="155" spans="2:71" ht="36" customHeight="1">
       <c r="B155" s="112"/>
-      <c r="C155" s="60" t="s">
-        <v>61</v>
+      <c r="C155" s="65" t="s">
+        <v>142</v>
       </c>
       <c r="D155" s="40"/>
       <c r="E155" s="41"/>
@@ -30318,10 +30324,10 @@
       <c r="BR155" s="4"/>
       <c r="BS155" s="4"/>
     </row>
-    <row r="156" spans="1:71" ht="36" customHeight="1">
+    <row r="156" spans="2:71" ht="36" customHeight="1">
       <c r="B156" s="112"/>
       <c r="C156" s="60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D156" s="40"/>
       <c r="E156" s="41"/>
@@ -30398,10 +30404,10 @@
       <c r="BR156" s="4"/>
       <c r="BS156" s="4"/>
     </row>
-    <row r="157" spans="1:71" ht="36" customHeight="1">
+    <row r="157" spans="2:71" ht="36" customHeight="1">
       <c r="B157" s="112"/>
       <c r="C157" s="60" t="s">
-        <v>145</v>
+        <v>61</v>
       </c>
       <c r="D157" s="40"/>
       <c r="E157" s="41"/>
@@ -30478,20 +30484,20 @@
       <c r="BR157" s="4"/>
       <c r="BS157" s="4"/>
     </row>
-    <row r="158" spans="1:71" ht="36" customHeight="1" thickBot="1">
-      <c r="B158" s="113"/>
-      <c r="C158" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D158" s="54"/>
-      <c r="E158" s="55"/>
-      <c r="F158" s="56">
+    <row r="158" spans="2:71" ht="36" customHeight="1">
+      <c r="B158" s="112"/>
+      <c r="C158" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="D158" s="40"/>
+      <c r="E158" s="41"/>
+      <c r="F158" s="42">
         <v>41</v>
       </c>
-      <c r="G158" s="56">
+      <c r="G158" s="42">
         <v>10</v>
       </c>
-      <c r="H158" s="57">
+      <c r="H158" s="45">
         <v>0</v>
       </c>
       <c r="I158" s="3"/>
@@ -30558,25 +30564,20 @@
       <c r="BR158" s="4"/>
       <c r="BS158" s="4"/>
     </row>
-    <row r="159" spans="1:71" ht="36" customHeight="1" thickTop="1">
-      <c r="A159" s="38"/>
-      <c r="B159" s="114"/>
-      <c r="C159" s="115" t="s">
-        <v>147</v>
-      </c>
-      <c r="D159" s="46" t="s">
-        <v>171</v>
-      </c>
-      <c r="E159" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="F159" s="48">
+    <row r="159" spans="2:71" ht="36" customHeight="1">
+      <c r="B159" s="112"/>
+      <c r="C159" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="D159" s="40"/>
+      <c r="E159" s="41"/>
+      <c r="F159" s="42">
         <v>41</v>
       </c>
-      <c r="G159" s="48">
+      <c r="G159" s="42">
         <v>10</v>
       </c>
-      <c r="H159" s="49">
+      <c r="H159" s="45">
         <v>0</v>
       </c>
       <c r="I159" s="3"/>
@@ -30643,20 +30644,20 @@
       <c r="BR159" s="4"/>
       <c r="BS159" s="4"/>
     </row>
-    <row r="160" spans="1:71" ht="36" customHeight="1">
-      <c r="B160" s="114"/>
-      <c r="C160" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="D160" s="40"/>
-      <c r="E160" s="41"/>
-      <c r="F160" s="42">
+    <row r="160" spans="2:71" ht="36" customHeight="1" thickBot="1">
+      <c r="B160" s="113"/>
+      <c r="C160" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D160" s="54"/>
+      <c r="E160" s="55"/>
+      <c r="F160" s="56">
         <v>41</v>
       </c>
-      <c r="G160" s="42">
+      <c r="G160" s="56">
         <v>10</v>
       </c>
-      <c r="H160" s="45">
+      <c r="H160" s="57">
         <v>0</v>
       </c>
       <c r="I160" s="3"/>
@@ -30723,20 +30724,25 @@
       <c r="BR160" s="4"/>
       <c r="BS160" s="4"/>
     </row>
-    <row r="161" spans="2:71" ht="36" customHeight="1">
+    <row r="161" spans="1:71" ht="36" customHeight="1" thickTop="1">
+      <c r="A161" s="38"/>
       <c r="B161" s="114"/>
-      <c r="C161" s="65" t="s">
-        <v>148</v>
-      </c>
-      <c r="D161" s="40"/>
-      <c r="E161" s="41"/>
-      <c r="F161" s="42">
+      <c r="C161" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="D161" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="E161" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="F161" s="48">
         <v>41</v>
       </c>
-      <c r="G161" s="42">
+      <c r="G161" s="48">
         <v>10</v>
       </c>
-      <c r="H161" s="45">
+      <c r="H161" s="49">
         <v>0</v>
       </c>
       <c r="I161" s="3"/>
@@ -30803,10 +30809,10 @@
       <c r="BR161" s="4"/>
       <c r="BS161" s="4"/>
     </row>
-    <row r="162" spans="2:71" ht="36" customHeight="1">
+    <row r="162" spans="1:71" ht="36" customHeight="1">
       <c r="B162" s="114"/>
       <c r="C162" s="65" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D162" s="40"/>
       <c r="E162" s="41"/>
@@ -30883,10 +30889,10 @@
       <c r="BR162" s="4"/>
       <c r="BS162" s="4"/>
     </row>
-    <row r="163" spans="2:71" ht="36" customHeight="1">
+    <row r="163" spans="1:71" ht="36" customHeight="1">
       <c r="B163" s="114"/>
       <c r="C163" s="65" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D163" s="40"/>
       <c r="E163" s="41"/>
@@ -30963,10 +30969,10 @@
       <c r="BR163" s="4"/>
       <c r="BS163" s="4"/>
     </row>
-    <row r="164" spans="2:71" ht="36" customHeight="1">
+    <row r="164" spans="1:71" ht="36" customHeight="1">
       <c r="B164" s="114"/>
-      <c r="C164" s="60" t="s">
-        <v>152</v>
+      <c r="C164" s="65" t="s">
+        <v>151</v>
       </c>
       <c r="D164" s="40"/>
       <c r="E164" s="41"/>
@@ -31043,10 +31049,10 @@
       <c r="BR164" s="4"/>
       <c r="BS164" s="4"/>
     </row>
-    <row r="165" spans="2:71" ht="36" customHeight="1">
+    <row r="165" spans="1:71" ht="36" customHeight="1">
       <c r="B165" s="114"/>
-      <c r="C165" s="60" t="s">
-        <v>153</v>
+      <c r="C165" s="65" t="s">
+        <v>150</v>
       </c>
       <c r="D165" s="40"/>
       <c r="E165" s="41"/>
@@ -31123,10 +31129,10 @@
       <c r="BR165" s="4"/>
       <c r="BS165" s="4"/>
     </row>
-    <row r="166" spans="2:71" ht="36" customHeight="1">
+    <row r="166" spans="1:71" ht="36" customHeight="1">
       <c r="B166" s="114"/>
       <c r="C166" s="60" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D166" s="40"/>
       <c r="E166" s="41"/>
@@ -31203,10 +31209,10 @@
       <c r="BR166" s="4"/>
       <c r="BS166" s="4"/>
     </row>
-    <row r="167" spans="2:71" ht="36" customHeight="1">
+    <row r="167" spans="1:71" ht="36" customHeight="1">
       <c r="B167" s="114"/>
       <c r="C167" s="60" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D167" s="40"/>
       <c r="E167" s="41"/>
@@ -31283,10 +31289,10 @@
       <c r="BR167" s="4"/>
       <c r="BS167" s="4"/>
     </row>
-    <row r="168" spans="2:71" ht="36" customHeight="1">
+    <row r="168" spans="1:71" ht="36" customHeight="1">
       <c r="B168" s="114"/>
       <c r="C168" s="60" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D168" s="40"/>
       <c r="E168" s="41"/>
@@ -31363,20 +31369,20 @@
       <c r="BR168" s="4"/>
       <c r="BS168" s="4"/>
     </row>
-    <row r="169" spans="2:71" ht="36" customHeight="1" thickBot="1">
+    <row r="169" spans="1:71" ht="36" customHeight="1">
       <c r="B169" s="114"/>
-      <c r="C169" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D169" s="54"/>
-      <c r="E169" s="55"/>
-      <c r="F169" s="56">
+      <c r="C169" s="60" t="s">
+        <v>155</v>
+      </c>
+      <c r="D169" s="40"/>
+      <c r="E169" s="41"/>
+      <c r="F169" s="42">
         <v>41</v>
       </c>
-      <c r="G169" s="56">
+      <c r="G169" s="42">
         <v>10</v>
       </c>
-      <c r="H169" s="57">
+      <c r="H169" s="45">
         <v>0</v>
       </c>
       <c r="I169" s="3"/>
@@ -31443,24 +31449,20 @@
       <c r="BR169" s="4"/>
       <c r="BS169" s="4"/>
     </row>
-    <row r="170" spans="2:71" ht="36" customHeight="1" thickTop="1">
-      <c r="B170" s="116"/>
-      <c r="C170" s="117" t="s">
+    <row r="170" spans="1:71" ht="36" customHeight="1">
+      <c r="B170" s="114"/>
+      <c r="C170" s="60" t="s">
+        <v>156</v>
+      </c>
+      <c r="D170" s="40"/>
+      <c r="E170" s="41"/>
+      <c r="F170" s="42">
         <v>41</v>
       </c>
-      <c r="D170" s="120" t="s">
-        <v>18</v>
-      </c>
-      <c r="E170" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="F170" s="48">
-        <v>41</v>
-      </c>
-      <c r="G170" s="48">
+      <c r="G170" s="42">
         <v>10</v>
       </c>
-      <c r="H170" s="49">
+      <c r="H170" s="45">
         <v>0</v>
       </c>
       <c r="I170" s="3"/>
@@ -31527,20 +31529,20 @@
       <c r="BR170" s="4"/>
       <c r="BS170" s="4"/>
     </row>
-    <row r="171" spans="2:71" ht="36" customHeight="1">
-      <c r="B171" s="118"/>
-      <c r="C171" s="65" t="s">
-        <v>157</v>
-      </c>
-      <c r="D171" s="40"/>
-      <c r="E171" s="41"/>
-      <c r="F171" s="42">
+    <row r="171" spans="1:71" ht="36" customHeight="1" thickBot="1">
+      <c r="B171" s="114"/>
+      <c r="C171" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D171" s="54"/>
+      <c r="E171" s="55"/>
+      <c r="F171" s="56">
         <v>41</v>
       </c>
-      <c r="G171" s="42">
+      <c r="G171" s="56">
         <v>10</v>
       </c>
-      <c r="H171" s="45">
+      <c r="H171" s="57">
         <v>0</v>
       </c>
       <c r="I171" s="3"/>
@@ -31607,20 +31609,24 @@
       <c r="BR171" s="4"/>
       <c r="BS171" s="4"/>
     </row>
-    <row r="172" spans="2:71" ht="36" customHeight="1">
-      <c r="B172" s="118"/>
-      <c r="C172" s="65" t="s">
-        <v>158</v>
-      </c>
-      <c r="D172" s="40"/>
-      <c r="E172" s="41"/>
-      <c r="F172" s="42">
+    <row r="172" spans="1:71" ht="36" customHeight="1" thickTop="1">
+      <c r="B172" s="116"/>
+      <c r="C172" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="G172" s="42">
+      <c r="D172" s="120" t="s">
+        <v>18</v>
+      </c>
+      <c r="E172" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="F172" s="48">
+        <v>41</v>
+      </c>
+      <c r="G172" s="48">
         <v>10</v>
       </c>
-      <c r="H172" s="45">
+      <c r="H172" s="49">
         <v>0</v>
       </c>
       <c r="I172" s="3"/>
@@ -31687,10 +31693,10 @@
       <c r="BR172" s="4"/>
       <c r="BS172" s="4"/>
     </row>
-    <row r="173" spans="2:71" ht="36" customHeight="1">
+    <row r="173" spans="1:71" ht="36" customHeight="1">
       <c r="B173" s="118"/>
       <c r="C173" s="65" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D173" s="40"/>
       <c r="E173" s="41"/>
@@ -31767,10 +31773,10 @@
       <c r="BR173" s="4"/>
       <c r="BS173" s="4"/>
     </row>
-    <row r="174" spans="2:71" ht="36" customHeight="1">
+    <row r="174" spans="1:71" ht="36" customHeight="1">
       <c r="B174" s="118"/>
       <c r="C174" s="65" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D174" s="40"/>
       <c r="E174" s="41"/>
@@ -31847,10 +31853,10 @@
       <c r="BR174" s="4"/>
       <c r="BS174" s="4"/>
     </row>
-    <row r="175" spans="2:71" ht="36" customHeight="1">
+    <row r="175" spans="1:71" ht="36" customHeight="1">
       <c r="B175" s="118"/>
-      <c r="C175" s="60" t="s">
-        <v>161</v>
+      <c r="C175" s="65" t="s">
+        <v>159</v>
       </c>
       <c r="D175" s="40"/>
       <c r="E175" s="41"/>
@@ -31927,10 +31933,10 @@
       <c r="BR175" s="4"/>
       <c r="BS175" s="4"/>
     </row>
-    <row r="176" spans="2:71" ht="36" customHeight="1">
+    <row r="176" spans="1:71" ht="36" customHeight="1">
       <c r="B176" s="118"/>
-      <c r="C176" s="60" t="s">
-        <v>162</v>
+      <c r="C176" s="65" t="s">
+        <v>160</v>
       </c>
       <c r="D176" s="40"/>
       <c r="E176" s="41"/>
@@ -32010,7 +32016,7 @@
     <row r="177" spans="2:71" ht="36" customHeight="1">
       <c r="B177" s="118"/>
       <c r="C177" s="60" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D177" s="40"/>
       <c r="E177" s="41"/>
@@ -32090,7 +32096,7 @@
     <row r="178" spans="2:71" ht="36" customHeight="1">
       <c r="B178" s="118"/>
       <c r="C178" s="60" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D178" s="40"/>
       <c r="E178" s="41"/>
@@ -32167,20 +32173,20 @@
       <c r="BR178" s="4"/>
       <c r="BS178" s="4"/>
     </row>
-    <row r="179" spans="2:71" ht="36" customHeight="1" thickBot="1">
-      <c r="B179" s="119"/>
-      <c r="C179" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D179" s="54"/>
-      <c r="E179" s="55"/>
-      <c r="F179" s="56">
+    <row r="179" spans="2:71" ht="36" customHeight="1">
+      <c r="B179" s="118"/>
+      <c r="C179" s="60" t="s">
+        <v>163</v>
+      </c>
+      <c r="D179" s="40"/>
+      <c r="E179" s="41"/>
+      <c r="F179" s="42">
         <v>41</v>
       </c>
-      <c r="G179" s="56">
+      <c r="G179" s="42">
         <v>10</v>
       </c>
-      <c r="H179" s="57">
+      <c r="H179" s="45">
         <v>0</v>
       </c>
       <c r="I179" s="3"/>
@@ -32247,7 +32253,167 @@
       <c r="BR179" s="4"/>
       <c r="BS179" s="4"/>
     </row>
-    <row r="180" spans="2:71" ht="30" customHeight="1" thickTop="1"/>
+    <row r="180" spans="2:71" ht="36" customHeight="1">
+      <c r="B180" s="118"/>
+      <c r="C180" s="60" t="s">
+        <v>164</v>
+      </c>
+      <c r="D180" s="40"/>
+      <c r="E180" s="41"/>
+      <c r="F180" s="42">
+        <v>41</v>
+      </c>
+      <c r="G180" s="42">
+        <v>10</v>
+      </c>
+      <c r="H180" s="45">
+        <v>0</v>
+      </c>
+      <c r="I180" s="3"/>
+      <c r="J180" s="3"/>
+      <c r="K180" s="3"/>
+      <c r="L180" s="3"/>
+      <c r="M180" s="3"/>
+      <c r="N180" s="3"/>
+      <c r="O180" s="3"/>
+      <c r="P180" s="3"/>
+      <c r="Q180" s="3"/>
+      <c r="R180" s="3"/>
+      <c r="S180" s="3"/>
+      <c r="T180" s="3"/>
+      <c r="U180" s="3"/>
+      <c r="V180" s="3"/>
+      <c r="W180" s="3"/>
+      <c r="X180" s="3"/>
+      <c r="Y180" s="3"/>
+      <c r="Z180" s="3"/>
+      <c r="AA180" s="3"/>
+      <c r="AB180" s="3"/>
+      <c r="AC180" s="4"/>
+      <c r="AD180" s="4"/>
+      <c r="AE180" s="4"/>
+      <c r="AF180" s="4"/>
+      <c r="AG180" s="4"/>
+      <c r="AH180" s="4"/>
+      <c r="AI180" s="4"/>
+      <c r="AJ180" s="4"/>
+      <c r="AK180" s="4"/>
+      <c r="AL180" s="4"/>
+      <c r="AM180" s="4"/>
+      <c r="AN180" s="4"/>
+      <c r="AO180" s="4"/>
+      <c r="AP180" s="4"/>
+      <c r="AQ180" s="4"/>
+      <c r="AR180" s="4"/>
+      <c r="AS180" s="4"/>
+      <c r="AT180" s="4"/>
+      <c r="AU180" s="4"/>
+      <c r="AV180" s="4"/>
+      <c r="AW180" s="4"/>
+      <c r="AX180" s="4"/>
+      <c r="AY180" s="4"/>
+      <c r="AZ180" s="4"/>
+      <c r="BA180" s="4"/>
+      <c r="BB180" s="4"/>
+      <c r="BC180" s="4"/>
+      <c r="BD180" s="4"/>
+      <c r="BE180" s="4"/>
+      <c r="BF180" s="4"/>
+      <c r="BG180" s="4"/>
+      <c r="BH180" s="4"/>
+      <c r="BI180" s="4"/>
+      <c r="BJ180" s="4"/>
+      <c r="BK180" s="4"/>
+      <c r="BL180" s="4"/>
+      <c r="BM180" s="4"/>
+      <c r="BN180" s="4"/>
+      <c r="BO180" s="4"/>
+      <c r="BP180" s="4"/>
+      <c r="BQ180" s="4"/>
+      <c r="BR180" s="4"/>
+      <c r="BS180" s="4"/>
+    </row>
+    <row r="181" spans="2:71" ht="36" customHeight="1" thickBot="1">
+      <c r="B181" s="119"/>
+      <c r="C181" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D181" s="54"/>
+      <c r="E181" s="55"/>
+      <c r="F181" s="56">
+        <v>41</v>
+      </c>
+      <c r="G181" s="56">
+        <v>10</v>
+      </c>
+      <c r="H181" s="57">
+        <v>0</v>
+      </c>
+      <c r="I181" s="3"/>
+      <c r="J181" s="3"/>
+      <c r="K181" s="3"/>
+      <c r="L181" s="3"/>
+      <c r="M181" s="3"/>
+      <c r="N181" s="3"/>
+      <c r="O181" s="3"/>
+      <c r="P181" s="3"/>
+      <c r="Q181" s="3"/>
+      <c r="R181" s="3"/>
+      <c r="S181" s="3"/>
+      <c r="T181" s="3"/>
+      <c r="U181" s="3"/>
+      <c r="V181" s="3"/>
+      <c r="W181" s="3"/>
+      <c r="X181" s="3"/>
+      <c r="Y181" s="3"/>
+      <c r="Z181" s="3"/>
+      <c r="AA181" s="3"/>
+      <c r="AB181" s="3"/>
+      <c r="AC181" s="4"/>
+      <c r="AD181" s="4"/>
+      <c r="AE181" s="4"/>
+      <c r="AF181" s="4"/>
+      <c r="AG181" s="4"/>
+      <c r="AH181" s="4"/>
+      <c r="AI181" s="4"/>
+      <c r="AJ181" s="4"/>
+      <c r="AK181" s="4"/>
+      <c r="AL181" s="4"/>
+      <c r="AM181" s="4"/>
+      <c r="AN181" s="4"/>
+      <c r="AO181" s="4"/>
+      <c r="AP181" s="4"/>
+      <c r="AQ181" s="4"/>
+      <c r="AR181" s="4"/>
+      <c r="AS181" s="4"/>
+      <c r="AT181" s="4"/>
+      <c r="AU181" s="4"/>
+      <c r="AV181" s="4"/>
+      <c r="AW181" s="4"/>
+      <c r="AX181" s="4"/>
+      <c r="AY181" s="4"/>
+      <c r="AZ181" s="4"/>
+      <c r="BA181" s="4"/>
+      <c r="BB181" s="4"/>
+      <c r="BC181" s="4"/>
+      <c r="BD181" s="4"/>
+      <c r="BE181" s="4"/>
+      <c r="BF181" s="4"/>
+      <c r="BG181" s="4"/>
+      <c r="BH181" s="4"/>
+      <c r="BI181" s="4"/>
+      <c r="BJ181" s="4"/>
+      <c r="BK181" s="4"/>
+      <c r="BL181" s="4"/>
+      <c r="BM181" s="4"/>
+      <c r="BN181" s="4"/>
+      <c r="BO181" s="4"/>
+      <c r="BP181" s="4"/>
+      <c r="BQ181" s="4"/>
+      <c r="BR181" s="4"/>
+      <c r="BS181" s="4"/>
+    </row>
+    <row r="182" spans="2:71" ht="30" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="G2:H2"/>
@@ -34549,7 +34715,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I108:BS108">
+  <conditionalFormatting sqref="I108:BS109">
     <cfRule type="expression" dxfId="471" priority="481">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34575,7 +34741,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I109:BS109">
+  <conditionalFormatting sqref="I110:BS110">
     <cfRule type="expression" dxfId="463" priority="473">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34601,7 +34767,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I110:BS110">
+  <conditionalFormatting sqref="I111:BS111">
     <cfRule type="expression" dxfId="455" priority="465">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34627,7 +34793,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I111:BS111">
+  <conditionalFormatting sqref="I112:BS112">
     <cfRule type="expression" dxfId="447" priority="457">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34653,7 +34819,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I112:BS112">
+  <conditionalFormatting sqref="I113:BS114">
     <cfRule type="expression" dxfId="439" priority="449">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34679,7 +34845,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I113:BS113">
+  <conditionalFormatting sqref="I115:BS115">
     <cfRule type="expression" dxfId="431" priority="441">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34705,7 +34871,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I114:BS114">
+  <conditionalFormatting sqref="I116:BS116">
     <cfRule type="expression" dxfId="423" priority="433">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34731,7 +34897,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I115:BS115">
+  <conditionalFormatting sqref="I117:BS117">
     <cfRule type="expression" dxfId="415" priority="425">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34757,7 +34923,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I116:BS116">
+  <conditionalFormatting sqref="I118:BS118">
     <cfRule type="expression" dxfId="407" priority="417">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34783,7 +34949,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I117:BS117">
+  <conditionalFormatting sqref="I119:BS119">
     <cfRule type="expression" dxfId="399" priority="409">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34809,7 +34975,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I118:BS119">
+  <conditionalFormatting sqref="I120:BS121">
     <cfRule type="expression" dxfId="391" priority="401">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34835,7 +35001,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I120:BS120">
+  <conditionalFormatting sqref="I122:BS122">
     <cfRule type="expression" dxfId="383" priority="393">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34861,7 +35027,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I121:BS121">
+  <conditionalFormatting sqref="I123:BS123">
     <cfRule type="expression" dxfId="375" priority="385">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34887,7 +35053,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I122:BS122">
+  <conditionalFormatting sqref="I124:BS124">
     <cfRule type="expression" dxfId="367" priority="377">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34913,7 +35079,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I123:BS124">
+  <conditionalFormatting sqref="I125:BS126">
     <cfRule type="expression" dxfId="359" priority="369">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34939,7 +35105,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I125:BS125">
+  <conditionalFormatting sqref="I127:BS127">
     <cfRule type="expression" dxfId="351" priority="361">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34965,7 +35131,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I126:BS126">
+  <conditionalFormatting sqref="I128:BS128">
     <cfRule type="expression" dxfId="343" priority="353">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -34991,7 +35157,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I127:BS127">
+  <conditionalFormatting sqref="I129:BS129">
     <cfRule type="expression" dxfId="335" priority="345">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35017,7 +35183,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I128:BS128">
+  <conditionalFormatting sqref="I130:BS130">
     <cfRule type="expression" dxfId="327" priority="337">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35043,7 +35209,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I129:BS129">
+  <conditionalFormatting sqref="I131:BS131">
     <cfRule type="expression" dxfId="319" priority="329">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35069,7 +35235,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I130:BS131">
+  <conditionalFormatting sqref="I132:BS133">
     <cfRule type="expression" dxfId="311" priority="321">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35095,7 +35261,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I159:BS159">
+  <conditionalFormatting sqref="I161:BS161">
     <cfRule type="expression" dxfId="303" priority="121">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35121,7 +35287,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I132:BS132">
+  <conditionalFormatting sqref="I134:BS134">
     <cfRule type="expression" dxfId="295" priority="305">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35147,7 +35313,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I133:BS133">
+  <conditionalFormatting sqref="I135:BS135">
     <cfRule type="expression" dxfId="287" priority="297">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35173,7 +35339,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I134:BS135">
+  <conditionalFormatting sqref="I136:BS137">
     <cfRule type="expression" dxfId="279" priority="289">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35199,7 +35365,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I168:BS168">
+  <conditionalFormatting sqref="I170:BS170">
     <cfRule type="expression" dxfId="271" priority="89">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35225,7 +35391,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I136:BS136">
+  <conditionalFormatting sqref="I138:BS138">
     <cfRule type="expression" dxfId="263" priority="273">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35251,7 +35417,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I137:BS137">
+  <conditionalFormatting sqref="I139:BS139">
     <cfRule type="expression" dxfId="255" priority="265">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35277,7 +35443,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I138:BS138">
+  <conditionalFormatting sqref="I140:BS140">
     <cfRule type="expression" dxfId="247" priority="257">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35303,7 +35469,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I139:BS139">
+  <conditionalFormatting sqref="I141:BS141">
     <cfRule type="expression" dxfId="239" priority="249">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35329,7 +35495,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I140:BS141">
+  <conditionalFormatting sqref="I142:BS143">
     <cfRule type="expression" dxfId="231" priority="241">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35355,7 +35521,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I142:BS142">
+  <conditionalFormatting sqref="I144:BS144">
     <cfRule type="expression" dxfId="223" priority="233">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35381,7 +35547,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I143:BS143">
+  <conditionalFormatting sqref="I145:BS145">
     <cfRule type="expression" dxfId="215" priority="225">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35407,7 +35573,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I144:BS144">
+  <conditionalFormatting sqref="I146:BS146">
     <cfRule type="expression" dxfId="207" priority="217">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35433,7 +35599,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I145:BS146">
+  <conditionalFormatting sqref="I147:BS148">
     <cfRule type="expression" dxfId="199" priority="209">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35459,7 +35625,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I147:BS147">
+  <conditionalFormatting sqref="I149:BS149">
     <cfRule type="expression" dxfId="191" priority="201">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35485,7 +35651,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I148:BS148">
+  <conditionalFormatting sqref="I150:BS150">
     <cfRule type="expression" dxfId="183" priority="193">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35511,7 +35677,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I149:BS149">
+  <conditionalFormatting sqref="I151:BS151">
     <cfRule type="expression" dxfId="175" priority="185">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35537,7 +35703,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I150:BS150">
+  <conditionalFormatting sqref="I152:BS152">
     <cfRule type="expression" dxfId="167" priority="177">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35563,7 +35729,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I151:BS151">
+  <conditionalFormatting sqref="I153:BS153">
     <cfRule type="expression" dxfId="159" priority="169">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35589,7 +35755,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I152:BS153">
+  <conditionalFormatting sqref="I154:BS155">
     <cfRule type="expression" dxfId="151" priority="161">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35615,7 +35781,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I154:BS154">
+  <conditionalFormatting sqref="I156:BS156">
     <cfRule type="expression" dxfId="143" priority="153">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35641,7 +35807,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I155:BS155">
+  <conditionalFormatting sqref="I157:BS157">
     <cfRule type="expression" dxfId="135" priority="145">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35667,7 +35833,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I156:BS157">
+  <conditionalFormatting sqref="I158:BS159">
     <cfRule type="expression" dxfId="127" priority="137">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35693,7 +35859,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I158:BS158">
+  <conditionalFormatting sqref="I160:BS160">
     <cfRule type="expression" dxfId="119" priority="129">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35719,7 +35885,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I160:BS162">
+  <conditionalFormatting sqref="I162:BS164">
     <cfRule type="expression" dxfId="111" priority="113">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35745,7 +35911,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I163:BS163">
+  <conditionalFormatting sqref="I165:BS165">
     <cfRule type="expression" dxfId="103" priority="105">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35771,7 +35937,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I164:BS164">
+  <conditionalFormatting sqref="I166:BS166">
     <cfRule type="expression" dxfId="95" priority="97">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35797,7 +35963,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I169:BS169">
+  <conditionalFormatting sqref="I171:BS171">
     <cfRule type="expression" dxfId="87" priority="81">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35823,7 +35989,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I165:BS165">
+  <conditionalFormatting sqref="I167:BS167">
     <cfRule type="expression" dxfId="79" priority="73">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35849,7 +36015,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I166:BS167">
+  <conditionalFormatting sqref="I168:BS169">
     <cfRule type="expression" dxfId="71" priority="65">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35875,7 +36041,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I170:BS170">
+  <conditionalFormatting sqref="I172:BS172">
     <cfRule type="expression" dxfId="63" priority="57">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35901,7 +36067,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I171:BS171">
+  <conditionalFormatting sqref="I173:BS173">
     <cfRule type="expression" dxfId="55" priority="49">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35927,7 +36093,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I172:BS172">
+  <conditionalFormatting sqref="I174:BS174">
     <cfRule type="expression" dxfId="47" priority="41">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35953,7 +36119,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I173:BS174">
+  <conditionalFormatting sqref="I175:BS176">
     <cfRule type="expression" dxfId="39" priority="33">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -35979,7 +36145,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I175:BS175">
+  <conditionalFormatting sqref="I177:BS177">
     <cfRule type="expression" dxfId="31" priority="25">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -36005,7 +36171,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I176:BS176">
+  <conditionalFormatting sqref="I178:BS178">
     <cfRule type="expression" dxfId="23" priority="17">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -36031,7 +36197,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I177:BS178">
+  <conditionalFormatting sqref="I179:BS180">
     <cfRule type="expression" dxfId="15" priority="9">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -36057,7 +36223,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I179:BS179">
+  <conditionalFormatting sqref="I181:BS181">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>

</xml_diff>

<commit_message>
[Modified]: meeting schedule sprint 2
</commit_message>
<xml_diff>
--- a/Báo Cáo/Activity_bar_chart và bảng phân hệ/Activity-bar-chart.xlsx
+++ b/Báo Cáo/Activity_bar_chart và bảng phân hệ/Activity-bar-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Software-Technology\Báo Cáo\Activity_bar_chart và bảng phân hệ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC277DD7-2C2E-42C0-8F8F-B369484EF19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCB0664-18A6-4F8B-BC8D-0A885C1AFB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17580,10 +17580,10 @@
   <dimension ref="A1:BT182"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="8" ySplit="5" topLeftCell="I105" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="8" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J114" sqref="J114"/>
+      <selection pane="bottomRight" activeCell="F186" sqref="F186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1"/>

</xml_diff>